<commit_message>
KKBOX autoint corr map + ieee_fraud_small_data_test
</commit_message>
<xml_diff>
--- a/data/KKBOX_summary.xlsx
+++ b/data/KKBOX_summary.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlitaNet\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD63D6EB-E2E7-40D7-AA80-462AAFB6F496}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933EE793-A450-406D-8310-A29F1FA2F7BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8CFFA5A3-4067-4660-B8C8-E79983DA0D55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="model reference" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1495,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ABD978-C0F8-4DC1-A89A-3B5F03A8407E}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F15" sqref="A1:F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1952,7 +1952,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
catboost benchmark on kkbox
</commit_message>
<xml_diff>
--- a/data/KKBOX_summary.xlsx
+++ b/data/KKBOX_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlitaNet\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933EE793-A450-406D-8310-A29F1FA2F7BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D4BB1E-410F-4D38-B903-8BC2C5E9C384}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8CFFA5A3-4067-4660-B8C8-E79983DA0D55}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>LR</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -192,6 +192,10 @@
   </si>
   <si>
     <t>By Franky</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CatBoost</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1493,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ABD978-C0F8-4DC1-A89A-3B5F03A8407E}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1555,7 @@
         <v>0.65900000000000003</v>
       </c>
       <c r="E2" s="3">
-        <f t="shared" ref="E2:E15" si="0">1000*(D2-0.6527)</f>
+        <f t="shared" ref="E2:E16" si="0">1000*(D2-0.6527)</f>
         <v>6.3000000000000833</v>
       </c>
       <c r="F2" s="2">
@@ -1562,7 +1566,7 @@
         <v>2.1875000000000289</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:H15" si="2">D2-C2</f>
+        <f t="shared" ref="H2:H16" si="2">D2-C2</f>
         <v>0</v>
       </c>
     </row>
@@ -1934,6 +1938,28 @@
       <c r="H15" s="1">
         <f t="shared" si="2"/>
         <v>5.6999999999999273E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.69450000000000001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.65439999999999998</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7000000000000348</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>-6.6000000000000503E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>